<commit_message>
train case 2 & 5 dof
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point_5dof.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point_5dof.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.008999999999999999</v>
+        <v>-0.26</v>
       </c>
       <c r="B1" t="n">
-        <v>0.103</v>
+        <v>-0.073</v>
       </c>
       <c r="C1" t="n">
-        <v>-0.328</v>
+        <v>-0.133</v>
       </c>
       <c r="D1" t="n">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="E1" t="n">
-        <v>-6</v>
+        <v>19</v>
       </c>
       <c r="F1" t="n">
-        <v>-161</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.329</v>
+        <v>0.114</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.235</v>
+        <v>0.172</v>
       </c>
       <c r="C2" t="n">
-        <v>0.11</v>
+        <v>0.507</v>
       </c>
       <c r="D2" t="n">
-        <v>-74</v>
+        <v>-89</v>
       </c>
       <c r="E2" t="n">
-        <v>20</v>
+        <v>-2</v>
       </c>
       <c r="F2" t="n">
-        <v>60</v>
+        <v>-164</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.111</v>
+        <v>0.172</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.131</v>
+        <v>-0.077</v>
       </c>
       <c r="C3" t="n">
-        <v>0.464</v>
+        <v>0.156</v>
       </c>
       <c r="D3" t="n">
-        <v>137</v>
+        <v>88</v>
       </c>
       <c r="E3" t="n">
-        <v>-78</v>
+        <v>86</v>
       </c>
       <c r="F3" t="n">
-        <v>-61</v>
+        <v>-172</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.015</v>
+        <v>-0.059</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.379</v>
+        <v>-0.222</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.145</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="D4" t="n">
-        <v>-50</v>
+        <v>108</v>
       </c>
       <c r="E4" t="n">
-        <v>-59</v>
+        <v>-10</v>
       </c>
       <c r="F4" t="n">
-        <v>59</v>
+        <v>-140</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.135</v>
+        <v>0.191</v>
       </c>
       <c r="B5" t="n">
-        <v>0.189</v>
+        <v>-0.379</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.044</v>
+        <v>0.238</v>
       </c>
       <c r="D5" t="n">
-        <v>154</v>
+        <v>16</v>
       </c>
       <c r="E5" t="n">
-        <v>-4</v>
+        <v>59</v>
       </c>
       <c r="F5" t="n">
-        <v>11</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.3</v>
+        <v>-0.196</v>
       </c>
       <c r="B6" t="n">
-        <v>0.109</v>
+        <v>-0.002</v>
       </c>
       <c r="C6" t="n">
-        <v>0.457</v>
+        <v>0.243</v>
       </c>
       <c r="D6" t="n">
-        <v>-130</v>
+        <v>-51</v>
       </c>
       <c r="E6" t="n">
-        <v>9</v>
+        <v>-49</v>
       </c>
       <c r="F6" t="n">
-        <v>61</v>
+        <v>-13</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.04</v>
+        <v>-0.093</v>
       </c>
       <c r="B7" t="n">
-        <v>0.244</v>
+        <v>0.24</v>
       </c>
       <c r="C7" t="n">
-        <v>0.149</v>
+        <v>0.472</v>
       </c>
       <c r="D7" t="n">
-        <v>-94</v>
+        <v>92</v>
       </c>
       <c r="E7" t="n">
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="F7" t="n">
-        <v>91</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-0.336</v>
+        <v>-0.2</v>
       </c>
       <c r="B8" t="n">
-        <v>0.019</v>
+        <v>-0.09</v>
       </c>
       <c r="C8" t="n">
-        <v>0.399</v>
+        <v>0.161</v>
       </c>
       <c r="D8" t="n">
-        <v>-112</v>
+        <v>115</v>
       </c>
       <c r="E8" t="n">
-        <v>-10</v>
+        <v>-36</v>
       </c>
       <c r="F8" t="n">
-        <v>-134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-0.057</v>
+        <v>0.116</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.342</v>
+        <v>-0.017</v>
       </c>
       <c r="C9" t="n">
-        <v>0.254</v>
+        <v>0.148</v>
       </c>
       <c r="D9" t="n">
-        <v>-121</v>
+        <v>-78</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>-7</v>
       </c>
       <c r="F9" t="n">
-        <v>10</v>
+        <v>-127</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.01</v>
+        <v>0.025</v>
       </c>
       <c r="B10" t="n">
-        <v>0.11</v>
+        <v>-0.135</v>
       </c>
       <c r="C10" t="n">
-        <v>0.421</v>
+        <v>0.158</v>
       </c>
       <c r="D10" t="n">
-        <v>-36</v>
+        <v>-95</v>
       </c>
       <c r="E10" t="n">
-        <v>-44</v>
+        <v>13</v>
       </c>
       <c r="F10" t="n">
-        <v>-37</v>
+        <v>-149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>